<commit_message>
fixed Sheet Name Error
</commit_message>
<xml_diff>
--- a/MergeAndCreatePivot/Daily Reports/Coffee Shop 1.xlsx
+++ b/MergeAndCreatePivot/Daily Reports/Coffee Shop 1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\calin.grigorescu\Documents\UiPath\ExcelConsolidation\Daily Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chego\OneDrive\Documents\UiPath\MergeAndCreatePivot\Daily Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC74FF8-4556-428A-9309-0E051F8DAF42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04CD7376-F645-421E-9376-420451CA1514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -416,15 +416,15 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -438,7 +438,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -453,7 +453,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -468,7 +468,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -483,7 +483,7 @@
         <v>423.5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -498,7 +498,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -513,7 +513,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -528,7 +528,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -543,7 +543,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -558,7 +558,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -573,7 +573,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>

</xml_diff>